<commit_message>
Start cleaning shu48 markups
</commit_message>
<xml_diff>
--- a/executables/LUDUMDARE/Notes/Notes.xlsx
+++ b/executables/LUDUMDARE/Notes/Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.hubart\Desktop\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Personnel\Programmation\Code\executables\LUDUMDARE\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7F079D-911F-4B89-9F64-D72B71D3E5A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2014A97-9359-4EEA-95B2-2D8ADD3A66C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21195" yWindow="1935" windowWidth="17505" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="360" windowWidth="24510" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>LD40</t>
   </si>
@@ -187,6 +187,18 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>LD48</t>
+  </si>
+  <si>
+    <t>Bouldaouf dash</t>
+  </si>
+  <si>
+    <t>2.603</t>
+  </si>
+  <si>
+    <t>2.735</t>
   </si>
 </sst>
 </file>
@@ -528,7 +540,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,15 +783,33 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3.2349999999999999</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.1030000000000002</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.7650000000000001</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2.8380000000000001</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2.758</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>